<commit_message>
Add new crawl projects of creators
</commit_message>
<xml_diff>
--- a/crawl_status.xlsx
+++ b/crawl_status.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="66">
   <si>
     <t>Category</t>
   </si>
@@ -54,151 +54,172 @@
     <t>project_id</t>
   </si>
   <si>
-    <t>tor_8</t>
-  </si>
-  <si>
-    <t>technology_3d_printing</t>
-  </si>
-  <si>
-    <t>technology_apps</t>
-  </si>
-  <si>
-    <t>technology_camera_equipment</t>
-  </si>
-  <si>
-    <t>technology_diy_electronics</t>
-  </si>
-  <si>
-    <t>technology_fabrication_tools</t>
-  </si>
-  <si>
-    <t>technology_flight</t>
-  </si>
-  <si>
-    <t>technology_gadgets</t>
-  </si>
-  <si>
-    <t>technology_hardware</t>
-  </si>
-  <si>
-    <t>technology_makerspaces</t>
-  </si>
-  <si>
-    <t>technology_robots</t>
-  </si>
-  <si>
-    <t>technology_software</t>
-  </si>
-  <si>
-    <t>technology_sound</t>
-  </si>
-  <si>
-    <t>technology_space_exploration</t>
-  </si>
-  <si>
-    <t>technology_wearables</t>
-  </si>
-  <si>
-    <t>technology_web</t>
-  </si>
-  <si>
-    <t>art_ceramics</t>
-  </si>
-  <si>
-    <t>art_conceptual</t>
-  </si>
-  <si>
-    <t>art_digital</t>
-  </si>
-  <si>
-    <t>art_illustration</t>
-  </si>
-  <si>
-    <t>art_installations</t>
-  </si>
-  <si>
-    <t>art_mixed_media</t>
-  </si>
-  <si>
-    <t>art_painting</t>
-  </si>
-  <si>
-    <t>art_performance</t>
-  </si>
-  <si>
-    <t>art_public</t>
-  </si>
-  <si>
-    <t>art_sculpture</t>
-  </si>
-  <si>
-    <t>art_social_practice</t>
-  </si>
-  <si>
-    <t>art_textiles</t>
-  </si>
-  <si>
-    <t>art_video_art</t>
-  </si>
-  <si>
-    <t>publishing_academic</t>
-  </si>
-  <si>
-    <t>publishing_anthologies</t>
-  </si>
-  <si>
-    <t>publishing_art_books</t>
-  </si>
-  <si>
-    <t>publishing_calendars</t>
-  </si>
-  <si>
-    <t>publishing_children_books</t>
-  </si>
-  <si>
-    <t>publishing_comedy</t>
-  </si>
-  <si>
-    <t>publishing_fiction</t>
-  </si>
-  <si>
-    <t>publishing_letterpress</t>
-  </si>
-  <si>
-    <t>publishing_literary_journals</t>
-  </si>
-  <si>
-    <t>publishing_literary_spaces</t>
-  </si>
-  <si>
-    <t>publishing_non_fictions</t>
-  </si>
-  <si>
-    <t>publishing_perodicals</t>
-  </si>
-  <si>
-    <t>publishing_peotry</t>
-  </si>
-  <si>
-    <t>publishing_radio_podcasts</t>
-  </si>
-  <si>
-    <t>publishing_tranlsations</t>
-  </si>
-  <si>
-    <t>publishing_young_adult</t>
-  </si>
-  <si>
-    <t>publishing_zines</t>
-  </si>
-  <si>
-    <t>tor_9</t>
-  </si>
-  <si>
-    <t>tor_10</t>
-  </si>
-  <si>
-    <t>tor_11</t>
+    <t>music_blues</t>
+  </si>
+  <si>
+    <t>music_chiptune</t>
+  </si>
+  <si>
+    <t>music_classical_music</t>
+  </si>
+  <si>
+    <t>music_comedy</t>
+  </si>
+  <si>
+    <t>music_country_folk</t>
+  </si>
+  <si>
+    <t>music_electronic_music</t>
+  </si>
+  <si>
+    <t>music_faith</t>
+  </si>
+  <si>
+    <t>music_hithop</t>
+  </si>
+  <si>
+    <t>music_indie_rock</t>
+  </si>
+  <si>
+    <t>music_jazz</t>
+  </si>
+  <si>
+    <t>music_kids</t>
+  </si>
+  <si>
+    <t>music_latin</t>
+  </si>
+  <si>
+    <t>music_metal</t>
+  </si>
+  <si>
+    <t>music_pop</t>
+  </si>
+  <si>
+    <t>music_punk</t>
+  </si>
+  <si>
+    <t>music_rb</t>
+  </si>
+  <si>
+    <t>music_rock</t>
+  </si>
+  <si>
+    <t>music_world</t>
+  </si>
+  <si>
+    <t>Fashion_accessories</t>
+  </si>
+  <si>
+    <t>Fashion_apparel</t>
+  </si>
+  <si>
+    <t>Fashion_childrenwear</t>
+  </si>
+  <si>
+    <t>Fashion_couture</t>
+  </si>
+  <si>
+    <t>Fashion_footwear</t>
+  </si>
+  <si>
+    <t>Fashion_jewelry</t>
+  </si>
+  <si>
+    <t>Fashion_pet</t>
+  </si>
+  <si>
+    <t>Fashion_ready_to_wear</t>
+  </si>
+  <si>
+    <t>crafts_candles</t>
+  </si>
+  <si>
+    <t>crafts_crochet</t>
+  </si>
+  <si>
+    <t>crafts_diy</t>
+  </si>
+  <si>
+    <t>crafts_embroidery</t>
+  </si>
+  <si>
+    <t>crafts_glass</t>
+  </si>
+  <si>
+    <t>crafts_knitting</t>
+  </si>
+  <si>
+    <t>crafts_pottery</t>
+  </si>
+  <si>
+    <t>crafts_printing</t>
+  </si>
+  <si>
+    <t>crafts_quilts</t>
+  </si>
+  <si>
+    <t>crafts_stationery</t>
+  </si>
+  <si>
+    <t>crafts_taxidermy</t>
+  </si>
+  <si>
+    <t>crafts_weaving</t>
+  </si>
+  <si>
+    <t>crafts_woodworking</t>
+  </si>
+  <si>
+    <t>food_bacon</t>
+  </si>
+  <si>
+    <t>food_community_gardens</t>
+  </si>
+  <si>
+    <t>food_cookbooks</t>
+  </si>
+  <si>
+    <t>food_drinks</t>
+  </si>
+  <si>
+    <t>food_event</t>
+  </si>
+  <si>
+    <t>food_farmer_markets</t>
+  </si>
+  <si>
+    <t>food_farm</t>
+  </si>
+  <si>
+    <t>food_trucks</t>
+  </si>
+  <si>
+    <t>food_restaurants</t>
+  </si>
+  <si>
+    <t>food_small_batch</t>
+  </si>
+  <si>
+    <t>food_spaces</t>
+  </si>
+  <si>
+    <t>food_vegan</t>
+  </si>
+  <si>
+    <t>kickstarter</t>
+  </si>
+  <si>
+    <t>tor_1</t>
+  </si>
+  <si>
+    <t>tor_2</t>
+  </si>
+  <si>
+    <t>tor_3</t>
+  </si>
+  <si>
+    <t>tor_4</t>
   </si>
 </sst>
 </file>
@@ -253,107 +274,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="59">
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="49">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -1120,16 +1041,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H82"/>
+  <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="I97" sqref="I97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="20.796875" customWidth="1"/>
     <col min="3" max="3" width="13.46484375" customWidth="1"/>
+    <col min="6" max="6" width="13.06640625" customWidth="1"/>
     <col min="7" max="7" width="17.59765625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1161,13 +1083,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
-        <v>331</v>
+        <v>316</v>
       </c>
       <c r="C2">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1176,21 +1098,18 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="C3">
-        <v>16</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1199,7 +1118,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
@@ -1207,13 +1126,13 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>332</v>
+        <v>36</v>
       </c>
       <c r="C4">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1222,7 +1141,7 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
@@ -1230,12 +1149,14 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <v>332</v>
+        <v>36</v>
       </c>
       <c r="C5">
-        <v>16</v>
-      </c>
-      <c r="D5" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E5">
         <v>1</v>
       </c>
@@ -1243,20 +1164,19 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6">
-        <v>333</v>
+        <v>36</v>
       </c>
       <c r="C6">
-        <v>16</v>
-      </c>
-      <c r="D6" s="3"/>
+        <v>14</v>
+      </c>
       <c r="E6">
         <v>1</v>
       </c>
@@ -1264,20 +1184,19 @@
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7">
-        <v>334</v>
+        <v>386</v>
       </c>
       <c r="C7">
-        <v>16</v>
-      </c>
-      <c r="D7" s="3"/>
+        <v>14</v>
+      </c>
       <c r="E7">
         <v>1</v>
       </c>
@@ -1285,20 +1204,22 @@
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8">
-        <v>335</v>
+        <v>37</v>
       </c>
       <c r="C8">
-        <v>16</v>
-      </c>
-      <c r="D8" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E8">
         <v>1</v>
       </c>
@@ -1306,20 +1227,22 @@
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9">
-        <v>336</v>
+        <v>37</v>
       </c>
       <c r="C9">
-        <v>16</v>
-      </c>
-      <c r="D9" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E9">
         <v>1</v>
       </c>
@@ -1327,21 +1250,18 @@
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B10">
-        <v>337</v>
+        <v>37</v>
       </c>
       <c r="C10">
-        <v>16</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -1350,21 +1270,21 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11">
-        <v>337</v>
+        <v>38</v>
       </c>
       <c r="C11">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -1373,20 +1293,22 @@
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12">
-        <v>337</v>
+        <v>38</v>
       </c>
       <c r="C12">
-        <v>16</v>
-      </c>
-      <c r="D12" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E12">
         <v>1</v>
       </c>
@@ -1394,21 +1316,18 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B13">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C13">
-        <v>16</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1417,21 +1336,18 @@
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B14">
-        <v>52</v>
+        <v>318</v>
       </c>
       <c r="C14">
-        <v>16</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -1440,20 +1356,22 @@
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C15">
-        <v>16</v>
-      </c>
-      <c r="D15" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E15">
         <v>1</v>
       </c>
@@ -1461,18 +1379,21 @@
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B16">
-        <v>362</v>
+        <v>39</v>
       </c>
       <c r="C16">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1481,18 +1402,18 @@
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B17">
-        <v>338</v>
+        <v>39</v>
       </c>
       <c r="C17">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -1501,18 +1422,18 @@
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B18">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C18">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>7</v>
@@ -1524,18 +1445,18 @@
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C19">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>6</v>
@@ -1547,18 +1468,18 @@
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C20">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1567,18 +1488,21 @@
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>339</v>
+        <v>41</v>
       </c>
       <c r="C21">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1587,20 +1511,22 @@
         <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B22">
-        <v>340</v>
+        <v>41</v>
       </c>
       <c r="C22">
-        <v>16</v>
-      </c>
-      <c r="D22" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E22">
         <v>1</v>
       </c>
@@ -1608,20 +1534,19 @@
         <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B23">
-        <v>341</v>
+        <v>41</v>
       </c>
       <c r="C23">
-        <v>16</v>
-      </c>
-      <c r="D23" s="3"/>
+        <v>14</v>
+      </c>
       <c r="E23">
         <v>1</v>
       </c>
@@ -1629,21 +1554,18 @@
         <v>0</v>
       </c>
       <c r="H23" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B24">
-        <v>342</v>
+        <v>319</v>
       </c>
       <c r="C24">
-        <v>16</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1652,21 +1574,18 @@
         <v>0</v>
       </c>
       <c r="H24" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B25">
-        <v>342</v>
+        <v>320</v>
       </c>
       <c r="C25">
-        <v>16</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1675,18 +1594,18 @@
         <v>0</v>
       </c>
       <c r="H25" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B26">
-        <v>342</v>
+        <v>241</v>
       </c>
       <c r="C26">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -1695,18 +1614,21 @@
         <v>0</v>
       </c>
       <c r="H26" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B27">
-        <v>287</v>
+        <v>42</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -1715,20 +1637,22 @@
         <v>0</v>
       </c>
       <c r="H27" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B28">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E28">
         <v>1</v>
       </c>
@@ -1736,18 +1660,18 @@
         <v>0</v>
       </c>
       <c r="H28" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B29">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -1756,21 +1680,18 @@
         <v>0</v>
       </c>
       <c r="H29" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B30">
-        <v>22</v>
+        <v>321</v>
       </c>
       <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -1779,21 +1700,18 @@
         <v>0</v>
       </c>
       <c r="H30" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B31">
-        <v>22</v>
+        <v>322</v>
       </c>
       <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -1802,18 +1720,21 @@
         <v>0</v>
       </c>
       <c r="H31" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B32">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -1822,18 +1743,21 @@
         <v>0</v>
       </c>
       <c r="H32" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B33">
-        <v>288</v>
+        <v>43</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -1842,21 +1766,18 @@
         <v>0</v>
       </c>
       <c r="H33" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B34">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -1865,21 +1786,21 @@
         <v>0</v>
       </c>
       <c r="H34" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B35">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -1888,18 +1809,21 @@
         <v>0</v>
       </c>
       <c r="H35" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B36">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C36">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -1908,21 +1832,18 @@
         <v>0</v>
       </c>
       <c r="H36" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B37">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="C37">
-        <v>1</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -1931,21 +1852,21 @@
         <v>0</v>
       </c>
       <c r="H37" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B38">
-        <v>23</v>
+        <v>262</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -1954,20 +1875,22 @@
         <v>0</v>
       </c>
       <c r="H38" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A39" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B39">
-        <v>23</v>
+        <v>262</v>
       </c>
       <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E39">
         <v>1</v>
       </c>
@@ -1975,20 +1898,19 @@
         <v>0</v>
       </c>
       <c r="H39" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B40">
-        <v>24</v>
+        <v>262</v>
       </c>
       <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="D40" s="3"/>
+        <v>9</v>
+      </c>
       <c r="E40">
         <v>1</v>
       </c>
@@ -1996,18 +1918,18 @@
         <v>0</v>
       </c>
       <c r="H40" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A41" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B41">
-        <v>53</v>
+        <v>263</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>7</v>
@@ -2019,18 +1941,18 @@
         <v>0</v>
       </c>
       <c r="H41" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B42">
-        <v>53</v>
+        <v>263</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>6</v>
@@ -2042,20 +1964,19 @@
         <v>0</v>
       </c>
       <c r="H42" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B43">
-        <v>53</v>
+        <v>263</v>
       </c>
       <c r="C43">
-        <v>1</v>
-      </c>
-      <c r="D43" s="3"/>
+        <v>9</v>
+      </c>
       <c r="E43">
         <v>1</v>
       </c>
@@ -2063,18 +1984,18 @@
         <v>0</v>
       </c>
       <c r="H43" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A44" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B44">
-        <v>25</v>
+        <v>264</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -2083,18 +2004,18 @@
         <v>0</v>
       </c>
       <c r="H44" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A45" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B45">
-        <v>395</v>
+        <v>265</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -2103,18 +2024,21 @@
         <v>0</v>
       </c>
       <c r="H45" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A46" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B46">
-        <v>289</v>
+        <v>266</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="E46">
         <v>1</v>
@@ -2123,18 +2047,21 @@
         <v>0</v>
       </c>
       <c r="H46" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A47" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B47">
-        <v>290</v>
+        <v>266</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -2143,18 +2070,18 @@
         <v>0</v>
       </c>
       <c r="H47" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A48" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B48">
-        <v>323</v>
+        <v>266</v>
       </c>
       <c r="C48">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -2163,18 +2090,18 @@
         <v>0</v>
       </c>
       <c r="H48" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B49">
-        <v>324</v>
+        <v>267</v>
       </c>
       <c r="C49">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E49">
         <v>1</v>
@@ -2183,21 +2110,18 @@
         <v>0</v>
       </c>
       <c r="H49" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A50" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B50">
-        <v>45</v>
+        <v>268</v>
       </c>
       <c r="C50">
-        <v>18</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E50">
         <v>1</v>
@@ -2206,21 +2130,18 @@
         <v>0</v>
       </c>
       <c r="H50" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B51">
-        <v>45</v>
+        <v>269</v>
       </c>
       <c r="C51">
-        <v>18</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E51">
         <v>1</v>
@@ -2229,18 +2150,18 @@
         <v>0</v>
       </c>
       <c r="H51" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A52" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B52">
-        <v>45</v>
+        <v>343</v>
       </c>
       <c r="C52">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E52">
         <v>1</v>
@@ -2249,18 +2170,18 @@
         <v>0</v>
       </c>
       <c r="H52" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A53" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B53">
-        <v>325</v>
+        <v>344</v>
       </c>
       <c r="C53">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E53">
         <v>1</v>
@@ -2269,21 +2190,18 @@
         <v>0</v>
       </c>
       <c r="H53" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A54" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B54">
-        <v>46</v>
+        <v>345</v>
       </c>
       <c r="C54">
-        <v>18</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E54">
         <v>1</v>
@@ -2292,21 +2210,18 @@
         <v>0</v>
       </c>
       <c r="H54" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B55">
-        <v>46</v>
+        <v>346</v>
       </c>
       <c r="C55">
-        <v>18</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="E55">
         <v>1</v>
@@ -2315,18 +2230,18 @@
         <v>0</v>
       </c>
       <c r="H55" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A56" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B56">
-        <v>46</v>
+        <v>347</v>
       </c>
       <c r="C56">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -2335,18 +2250,18 @@
         <v>0</v>
       </c>
       <c r="H56" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A57" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B57">
-        <v>387</v>
+        <v>348</v>
       </c>
       <c r="C57">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E57">
         <v>1</v>
@@ -2355,21 +2270,18 @@
         <v>0</v>
       </c>
       <c r="H57" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A58" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B58">
-        <v>47</v>
+        <v>350</v>
       </c>
       <c r="C58">
-        <v>18</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -2378,21 +2290,18 @@
         <v>0</v>
       </c>
       <c r="H58" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A59" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B59">
-        <v>47</v>
+        <v>351</v>
       </c>
       <c r="C59">
-        <v>18</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="E59">
         <v>1</v>
@@ -2401,18 +2310,18 @@
         <v>0</v>
       </c>
       <c r="H59" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A60" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B60">
-        <v>47</v>
+        <v>352</v>
       </c>
       <c r="C60">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E60">
         <v>1</v>
@@ -2421,18 +2330,18 @@
         <v>0</v>
       </c>
       <c r="H60" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B61">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="C61">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -2441,18 +2350,18 @@
         <v>0</v>
       </c>
       <c r="H61" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A62" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B62">
-        <v>326</v>
+        <v>354</v>
       </c>
       <c r="C62">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -2461,18 +2370,18 @@
         <v>0</v>
       </c>
       <c r="H62" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A63" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B63">
-        <v>389</v>
+        <v>355</v>
       </c>
       <c r="C63">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E63">
         <v>1</v>
@@ -2481,21 +2390,18 @@
         <v>0</v>
       </c>
       <c r="H63" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A64" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B64">
-        <v>48</v>
+        <v>356</v>
       </c>
       <c r="C64">
-        <v>18</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E64">
         <v>1</v>
@@ -2504,7 +2410,7 @@
         <v>0</v>
       </c>
       <c r="H64" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.45">
@@ -2512,13 +2418,10 @@
         <v>49</v>
       </c>
       <c r="B65">
-        <v>48</v>
+        <v>304</v>
       </c>
       <c r="C65">
-        <v>18</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E65">
         <v>1</v>
@@ -2527,18 +2430,18 @@
         <v>0</v>
       </c>
       <c r="H65" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A66" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B66">
-        <v>48</v>
+        <v>305</v>
       </c>
       <c r="C66">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E66">
         <v>1</v>
@@ -2547,21 +2450,18 @@
         <v>0</v>
       </c>
       <c r="H66" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A67" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B67">
-        <v>49</v>
+        <v>306</v>
       </c>
       <c r="C67">
-        <v>18</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E67">
         <v>1</v>
@@ -2570,21 +2470,21 @@
         <v>0</v>
       </c>
       <c r="H67" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A68" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B68">
-        <v>49</v>
+        <v>307</v>
       </c>
       <c r="C68">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E68">
         <v>1</v>
@@ -2593,18 +2493,21 @@
         <v>0</v>
       </c>
       <c r="H68" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A69" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B69">
-        <v>49</v>
+        <v>307</v>
       </c>
       <c r="C69">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -2613,18 +2516,18 @@
         <v>0</v>
       </c>
       <c r="H69" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A70" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B70">
-        <v>50</v>
+        <v>307</v>
       </c>
       <c r="C70">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E70">
         <v>1</v>
@@ -2633,18 +2536,18 @@
         <v>0</v>
       </c>
       <c r="H70" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A71" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B71">
-        <v>239</v>
+        <v>308</v>
       </c>
       <c r="C71">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E71">
         <v>1</v>
@@ -2653,18 +2556,18 @@
         <v>0</v>
       </c>
       <c r="H71" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A72" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B72">
-        <v>327</v>
+        <v>310</v>
       </c>
       <c r="C72">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -2673,18 +2576,18 @@
         <v>0</v>
       </c>
       <c r="H72" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A73" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B73">
-        <v>328</v>
+        <v>309</v>
       </c>
       <c r="C73">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E73">
         <v>1</v>
@@ -2693,18 +2596,21 @@
         <v>0</v>
       </c>
       <c r="H73" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B74">
-        <v>329</v>
+        <v>311</v>
       </c>
       <c r="C74">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="E74">
         <v>1</v>
@@ -2713,305 +2619,482 @@
         <v>0</v>
       </c>
       <c r="H74" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A75" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B75">
+        <v>311</v>
+      </c>
+      <c r="C75">
+        <v>10</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E75">
+        <v>1</v>
+      </c>
+      <c r="G75" t="b">
+        <v>0</v>
+      </c>
+      <c r="H75" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A76" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B76">
+        <v>311</v>
+      </c>
+      <c r="C76">
+        <v>10</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="G76" t="b">
+        <v>0</v>
+      </c>
+      <c r="H76" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A77" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B77">
+        <v>312</v>
+      </c>
+      <c r="C77">
+        <v>10</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
+      <c r="G77" t="b">
+        <v>0</v>
+      </c>
+      <c r="H77" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A78" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B78">
+        <v>312</v>
+      </c>
+      <c r="C78">
+        <v>10</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+      <c r="G78" t="b">
+        <v>0</v>
+      </c>
+      <c r="H78" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A79" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B79">
+        <v>312</v>
+      </c>
+      <c r="C79">
+        <v>10</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+      <c r="G79" t="b">
+        <v>0</v>
+      </c>
+      <c r="H79" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A80" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A82" s="2"/>
+      <c r="B80">
+        <v>313</v>
+      </c>
+      <c r="C80">
+        <v>10</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
+      <c r="G80" t="b">
+        <v>0</v>
+      </c>
+      <c r="H80" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A81" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B81">
+        <v>313</v>
+      </c>
+      <c r="C81">
+        <v>10</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
+      <c r="G81" t="b">
+        <v>0</v>
+      </c>
+      <c r="H81" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A82" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B82">
+        <v>313</v>
+      </c>
+      <c r="C82">
+        <v>10</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+      <c r="G82" t="b">
+        <v>0</v>
+      </c>
+      <c r="H82" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A83" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B83">
+        <v>314</v>
+      </c>
+      <c r="C83">
+        <v>10</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+      <c r="G83" t="b">
+        <v>0</v>
+      </c>
+      <c r="H83" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A84" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B84">
+        <v>315</v>
+      </c>
+      <c r="C84">
+        <v>10</v>
+      </c>
+      <c r="E84">
+        <v>1</v>
+      </c>
+      <c r="G84" t="b">
+        <v>0</v>
+      </c>
+      <c r="H84" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A85" s="2"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A86" s="2"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A87" s="2"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A88" s="2"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A89" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H1"/>
-  <conditionalFormatting sqref="G1:G2 G78:G82 G27 G88:G1048576">
-    <cfRule type="cellIs" dxfId="58" priority="81" operator="equal">
+  <conditionalFormatting sqref="G1 G90:G1048576">
+    <cfRule type="cellIs" dxfId="48" priority="137" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2">
+    <cfRule type="cellIs" dxfId="47" priority="56" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3">
+    <cfRule type="cellIs" dxfId="46" priority="55" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4">
+    <cfRule type="cellIs" dxfId="45" priority="54" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5">
+    <cfRule type="cellIs" dxfId="44" priority="53" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6">
+    <cfRule type="cellIs" dxfId="43" priority="52" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="cellIs" dxfId="57" priority="54" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G31">
-    <cfRule type="cellIs" dxfId="56" priority="40" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="55" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="51" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
+    <cfRule type="cellIs" dxfId="41" priority="50" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G9">
+    <cfRule type="cellIs" dxfId="40" priority="49" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10">
+    <cfRule type="cellIs" dxfId="39" priority="48" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11">
+    <cfRule type="cellIs" dxfId="38" priority="47" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12">
+    <cfRule type="cellIs" dxfId="37" priority="46" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13">
+    <cfRule type="cellIs" dxfId="36" priority="45" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G14">
+    <cfRule type="cellIs" dxfId="35" priority="44" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G15">
+    <cfRule type="cellIs" dxfId="34" priority="43" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G16">
+    <cfRule type="cellIs" dxfId="33" priority="42" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G17">
+    <cfRule type="cellIs" dxfId="32" priority="41" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G18">
+    <cfRule type="cellIs" dxfId="31" priority="40" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G19">
+    <cfRule type="cellIs" dxfId="30" priority="39" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G20">
+    <cfRule type="cellIs" dxfId="29" priority="38" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G21">
+    <cfRule type="cellIs" dxfId="28" priority="37" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G22">
+    <cfRule type="cellIs" dxfId="27" priority="36" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G23">
+    <cfRule type="cellIs" dxfId="26" priority="35" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G24">
+    <cfRule type="cellIs" dxfId="25" priority="34" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G25">
+    <cfRule type="cellIs" dxfId="24" priority="33" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26">
-    <cfRule type="cellIs" dxfId="54" priority="42" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G3">
-    <cfRule type="cellIs" dxfId="53" priority="58" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G21:G24">
-    <cfRule type="cellIs" dxfId="52" priority="44" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G39">
-    <cfRule type="cellIs" dxfId="51" priority="33" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G20">
-    <cfRule type="cellIs" dxfId="50" priority="45" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G4">
-    <cfRule type="cellIs" dxfId="49" priority="57" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G41">
-    <cfRule type="cellIs" dxfId="48" priority="31" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="47" priority="55" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G33:G34">
-    <cfRule type="cellIs" dxfId="46" priority="38" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G8:G10">
-    <cfRule type="cellIs" dxfId="45" priority="53" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G11">
-    <cfRule type="cellIs" dxfId="44" priority="52" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G12">
-    <cfRule type="cellIs" dxfId="43" priority="51" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G13">
-    <cfRule type="cellIs" dxfId="42" priority="50" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G14">
-    <cfRule type="cellIs" dxfId="41" priority="49" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G15">
-    <cfRule type="cellIs" dxfId="40" priority="48" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G16:G18">
-    <cfRule type="cellIs" dxfId="39" priority="47" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G19">
-    <cfRule type="cellIs" dxfId="38" priority="46" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G25">
-    <cfRule type="cellIs" dxfId="37" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="32" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G27">
+    <cfRule type="cellIs" dxfId="22" priority="31" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G28">
+    <cfRule type="cellIs" dxfId="21" priority="30" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G29">
+    <cfRule type="cellIs" dxfId="20" priority="29" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G30:G37">
+    <cfRule type="cellIs" dxfId="19" priority="28" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G38">
-    <cfRule type="cellIs" dxfId="36" priority="34" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G28:G30">
-    <cfRule type="cellIs" dxfId="35" priority="41" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G43">
-    <cfRule type="cellIs" dxfId="34" priority="29" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G32">
-    <cfRule type="cellIs" dxfId="33" priority="39" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G35">
-    <cfRule type="cellIs" dxfId="32" priority="37" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G36">
-    <cfRule type="cellIs" dxfId="31" priority="36" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G37">
-    <cfRule type="cellIs" dxfId="30" priority="35" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G40">
-    <cfRule type="cellIs" dxfId="29" priority="32" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G42">
-    <cfRule type="cellIs" dxfId="28" priority="30" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G44">
-    <cfRule type="cellIs" dxfId="27" priority="28" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G45">
-    <cfRule type="cellIs" dxfId="26" priority="27" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G46:G47">
-    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G48">
-    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G49">
-    <cfRule type="cellIs" dxfId="23" priority="24" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G50">
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="27" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G39:G50">
+    <cfRule type="cellIs" dxfId="17" priority="26" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51">
-    <cfRule type="cellIs" dxfId="21" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="25" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G52">
-    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G53">
-    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G54">
-    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G55">
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G56">
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G57">
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G58">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G59">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G60">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G61">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G62">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G63">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G64">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="24" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G53:G62">
+    <cfRule type="cellIs" dxfId="14" priority="23" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G63:G64">
+    <cfRule type="cellIs" dxfId="13" priority="22" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G65">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G66">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G67">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G68">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="19" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G66:G68">
+    <cfRule type="cellIs" dxfId="11" priority="18" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G69">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="17" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G70">
+    <cfRule type="cellIs" dxfId="9" priority="16" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G71:G73">
+    <cfRule type="cellIs" dxfId="8" priority="15" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G74">
+    <cfRule type="cellIs" dxfId="7" priority="14" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G75">
+    <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G76:G78">
+    <cfRule type="cellIs" dxfId="5" priority="12" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G79">
+    <cfRule type="cellIs" dxfId="4" priority="11" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G80">
+    <cfRule type="cellIs" dxfId="3" priority="10" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G81">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G71">
+  <conditionalFormatting sqref="G82">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G72:G74">
+  <conditionalFormatting sqref="G83:G89">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>

</xml_diff>